<commit_message>
Updated to use work items
</commit_message>
<xml_diff>
--- a/input_files/FindNewsInput.xlsx
+++ b/input_files/FindNewsInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Victor\robocorp\news_scraping\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00A2096-C9D5-48D6-8E58-94AF3071094E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC25C20E-573E-42C3-95DF-1F27BA26F954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foaie1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>score</t>
   </si>
   <si>
-    <t>Features</t>
+    <t>Sport</t>
   </si>
 </sst>
 </file>
@@ -359,9 +359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -398,5 +396,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>